<commit_message>
Fix bugs in uc-a-01
</commit_message>
<xml_diff>
--- a/phase2_use_cases/questions.xlsx
+++ b/phase2_use_cases/questions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Информационна система за управление на зали</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>uc-a-01 dali tova s mobilnoto prilojenie e OK UC</t>
   </si>
 </sst>
 </file>
@@ -458,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,6 +627,11 @@
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>